<commit_message>
HG-329 AEF: Excel and CSV Report genration
</commit_message>
<xml_diff>
--- a/backend/services/libs/shared/src/templates/aef_actions_template.xlsx
+++ b/backend/services/libs/shared/src/templates/aef_actions_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AmilaDissanayake\Projects\carbon-registry-undp\carbon-registry-zim\backend\services\libs\shared\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8109BF20-598D-4AEC-92E4-720390C11DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA94FBB4-7563-47B2-AADB-9E08607A52DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4A6097B3-A9B2-43A8-BF23-64D8708A96D2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4A6097B3-A9B2-43A8-BF23-64D8708A96D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="1" r:id="rId1"/>
@@ -129,13 +129,55 @@
     <t>Underlying unit block start ID</t>
   </si>
   <si>
-    <t>Underlying unit last block end</t>
-  </si>
-  <si>
     <t>Metric</t>
   </si>
   <si>
     <t>Quantity (expressed in metric)</t>
+  </si>
+  <si>
+    <t>First transferring participating Party</t>
+  </si>
+  <si>
+    <t>Vintage</t>
+  </si>
+  <si>
+    <t>Sector(s)</t>
+  </si>
+  <si>
+    <t>Activity type(s)</t>
+  </si>
+  <si>
+    <t>Date of authorization</t>
+  </si>
+  <si>
+    <t>Authorization ID</t>
+  </si>
+  <si>
+    <t>OIMP authorized by the Party</t>
+  </si>
+  <si>
+    <t>Action date</t>
+  </si>
+  <si>
+    <t>First transfer definition</t>
+  </si>
+  <si>
+    <t>Action type</t>
+  </si>
+  <si>
+    <t>Transferring participating Party</t>
+  </si>
+  <si>
+    <t>Acquiring participating Party</t>
+  </si>
+  <si>
+    <t>Purposes for cancellation</t>
+  </si>
+  <si>
+    <t>First transfer</t>
+  </si>
+  <si>
+    <t>Underlying unit last block end ID</t>
   </si>
   <si>
     <r>
@@ -143,6 +185,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="8"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
@@ -152,6 +195,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <i/>
         <sz val="8"/>
         <color rgb="FF000000"/>
@@ -161,73 +205,18 @@
       <t>(reporting Party)</t>
     </r>
   </si>
-  <si>
-    <t>First transferring participating Party</t>
-  </si>
-  <si>
-    <t>Vintage</t>
-  </si>
-  <si>
-    <t>Sector(s)</t>
-  </si>
-  <si>
-    <t>Activity type(s)</t>
-  </si>
-  <si>
-    <t>Date of authorization</t>
-  </si>
-  <si>
-    <t>Authorization ID</t>
-  </si>
-  <si>
-    <t>OIMP authorized by the Party</t>
-  </si>
-  <si>
-    <t>Action date</t>
-  </si>
-  <si>
-    <t>First transfer definition</t>
-  </si>
-  <si>
-    <t>Action type</t>
-  </si>
-  <si>
-    <t>Transferring participating Party</t>
-  </si>
-  <si>
-    <t>Acquiring participating Party</t>
-  </si>
-  <si>
-    <t>Purposes for cancellation</t>
-  </si>
-  <si>
-    <t>First transfer</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -286,10 +275,10 @@
     </font>
     <font>
       <b/>
-      <i/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -382,70 +371,65 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -763,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3990E1-B746-4A17-985C-D040B9086346}">
   <dimension ref="A2:Z34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="M2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,29 +783,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
+      <c r="B2" s="9"/>
     </row>
     <row r="3" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -830,227 +814,228 @@
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="19" t="s">
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="T8" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
+    </row>
+    <row r="9" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="21"/>
+    </row>
+    <row r="10" spans="1:26" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S10" s="16"/>
+      <c r="T10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="V10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="T8" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="U8" s="22"/>
-      <c r="V8" s="22"/>
-      <c r="W8" s="22"/>
-      <c r="X8" s="22"/>
-      <c r="Y8" s="22"/>
-      <c r="Z8" s="22"/>
-    </row>
-    <row r="9" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="23"/>
-    </row>
-    <row r="10" spans="1:26" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="M10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="N10" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P10" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q10" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="R10" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="S10" s="21"/>
-      <c r="T10" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="U10" s="13" t="s">
+      <c r="W10" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="V10" s="17" t="s">
+      <c r="X10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="W10" s="13" t="s">
+      <c r="Y10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="X10" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y10" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z10" s="13" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
+      <c r="A11" s="4"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
+      <c r="A12" s="4"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
+      <c r="A13" s="4"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
+      <c r="A14" s="13"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
+      <c r="A15" s="4"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
+      <c r="A16" s="4"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
+      <c r="A17" s="4"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
+      <c r="A18" s="4"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
+      <c r="A19" s="13"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
+      <c r="A20" s="4"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
+      <c r="A21" s="4"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
+      <c r="A22" s="4"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
+      <c r="A23" s="4"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
+      <c r="A24" s="4"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
+      <c r="A25" s="4"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
+      <c r="A26" s="4"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="6"/>
+      <c r="A27" s="4"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6"/>
+      <c r="A28" s="4"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="6"/>
+      <c r="A29" s="4"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="6"/>
+      <c r="A30" s="4"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="6"/>
+      <c r="A31" s="4"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="6"/>
+      <c r="A32" s="4"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="6"/>
+      <c r="A33" s="4"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
@@ -1074,6 +1059,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f3801cd2-1656-42b6-a361-01c162c981d7" xsi:nil="true"/>
@@ -1082,15 +1076,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1323,20 +1308,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EECD39DE-2373-4013-BB1A-947D9C34A5ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23AE2432-8CDD-42B8-8ACB-9372317A0BFE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="f3801cd2-1656-42b6-a361-01c162c981d7"/>
     <ds:schemaRef ds:uri="6d8fda5c-05ec-4e71-ae39-42f33d20b2eb"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EECD39DE-2373-4013-BB1A-947D9C34A5ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
aef last bloack id title rename
</commit_message>
<xml_diff>
--- a/backend/services/libs/shared/src/templates/aef_actions_template.xlsx
+++ b/backend/services/libs/shared/src/templates/aef_actions_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AmilaDissanayake\Projects\carbon-registry-undp\carbon-registry-zim\backend\services\libs\shared\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA94FBB4-7563-47B2-AADB-9E08607A52DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3347C08B-5C67-4EB4-B990-DDF3BB4818DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4A6097B3-A9B2-43A8-BF23-64D8708A96D2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4A6097B3-A9B2-43A8-BF23-64D8708A96D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="1" r:id="rId1"/>
@@ -177,9 +177,6 @@
     <t>First transfer</t>
   </si>
   <si>
-    <t>Underlying unit last block end ID</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Conversion factor </t>
     </r>
@@ -204,6 +201,9 @@
       </rPr>
       <t>(reporting Party)</t>
     </r>
+  </si>
+  <si>
+    <t>Underlying unit block last ID</t>
   </si>
 </sst>
 </file>
@@ -407,29 +407,29 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -747,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3990E1-B746-4A17-985C-D040B9086346}">
   <dimension ref="A2:Z34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -819,95 +819,95 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="18"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="14"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
       <c r="R8" s="12"/>
-      <c r="S8" s="14" t="s">
+      <c r="S8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="T8" s="17" t="s">
+      <c r="T8" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17"/>
-      <c r="W8" s="17"/>
-      <c r="X8" s="17"/>
-      <c r="Y8" s="17"/>
-      <c r="Z8" s="17"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="21"/>
     </row>
     <row r="9" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="17" t="s">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17" t="s">
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17" t="s">
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="19" t="s">
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="20" t="s">
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="U9" s="20"/>
-      <c r="V9" s="20"/>
-      <c r="W9" s="20"/>
-      <c r="X9" s="20"/>
-      <c r="Y9" s="20"/>
-      <c r="Z9" s="21"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="15"/>
     </row>
     <row r="10" spans="1:26" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="22" t="s">
-        <v>37</v>
+      <c r="F10" s="16" t="s">
+        <v>38</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>21</v>
@@ -919,7 +919,7 @@
         <v>12</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K10" s="11" t="s">
         <v>23</v>
@@ -945,7 +945,7 @@
       <c r="R10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="S10" s="16"/>
+      <c r="S10" s="20"/>
       <c r="T10" s="11" t="s">
         <v>30</v>
       </c>

</xml_diff>